<commit_message>
Maj color travail préparatoire
</commit_message>
<xml_diff>
--- a/Travail_Préparatoire.xlsx
+++ b/Travail_Préparatoire.xlsx
@@ -935,7 +935,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -964,6 +964,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF356854"/>
         <bgColor rgb="FF356854"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF11734B"/>
+        <bgColor rgb="FF11734B"/>
       </patternFill>
     </fill>
     <fill>
@@ -2336,86 +2342,86 @@
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="11" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="46" fillId="3" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="46" fillId="6" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="3" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="6" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="11" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="11" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="7" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="46" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="46" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="11" fillId="9" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="9" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="9" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="46" fillId="8" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="46" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="11" fillId="6" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="7" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="9" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="9" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="60" fillId="6" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="60" fillId="7" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="60" fillId="0" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -2481,30 +2487,30 @@
     <xf borderId="0" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="74" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="74" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="75" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="75" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="76" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="76" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="77" fillId="0" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="74" fillId="0" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="75" fillId="8" fontId="33" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="75" fillId="9" fontId="33" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="75" fillId="8" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="75" fillId="9" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="75" fillId="8" fontId="33" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="75" fillId="9" fontId="33" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="33" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="9" fontId="33" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2517,163 +2523,139 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="78" fillId="0" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="75" fillId="8" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="75" fillId="9" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="75" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="75" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="76" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="76" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="9" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="9" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="9" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="8" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="9" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="79" fillId="0" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="7" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="7" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="7" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="7" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="10" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="46" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="46" fillId="10" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="9" fontId="33" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="10" fontId="33" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="9" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="10" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="9" fontId="33" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="10" fontId="33" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="10" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="9" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="10" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="10" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="11" fillId="11" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="11" fontId="26" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="11" fontId="26" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="74" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="75" fillId="9" fontId="33" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="80" fillId="9" fontId="33" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="80" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="81" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="82" fillId="0" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="83" fillId="0" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="80" fillId="9" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="80" fillId="9" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="80" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="81" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="11" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="10" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="10" fontId="26" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="10" fontId="26" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="74" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="82" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="74" fillId="10" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="75" fillId="8" fontId="33" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="75" fillId="10" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="76" fillId="10" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="75" fillId="10" fontId="33" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="80" fillId="8" fontId="33" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="75" fillId="10" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="75" fillId="10" fontId="33" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="80" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="81" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="82" fillId="0" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="83" fillId="0" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="80" fillId="8" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="80" fillId="8" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="80" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="81" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="82" fillId="8" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="74" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="75" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="76" fillId="9" fontId="33" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="75" fillId="9" fontId="33" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="75" fillId="9" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="75" fillId="9" fontId="33" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="9" fontId="33" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="11" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="74" fillId="11" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="75" fillId="11" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="76" fillId="11" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="75" fillId="11" fontId="34" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="75" fillId="11" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="75" fillId="11" fontId="34" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="11" fontId="34" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="10" fontId="33" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="11" fillId="12" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -2683,36 +2665,60 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="75" fillId="12" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="76" fillId="12" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="75" fillId="12" fontId="34" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="75" fillId="12" fontId="34" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="75" fillId="12" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="75" fillId="12" fontId="34" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="75" fillId="12" fontId="34" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="76" fillId="12" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="11" fillId="12" fontId="34" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="81" fillId="12" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="13" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="74" fillId="13" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="75" fillId="13" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="76" fillId="13" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="75" fillId="13" fontId="34" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="75" fillId="13" fontId="34" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="75" fillId="13" fontId="34" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="75" fillId="13" fontId="34" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="76" fillId="13" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="10" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="13" fontId="34" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="81" fillId="13" fontId="34" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="11" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="11" fillId="10" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="11" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>

</xml_diff>